<commit_message>
created defaulters, UI changes for other pages
</commit_message>
<xml_diff>
--- a/product backlog.xlsx
+++ b/product backlog.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="issues" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>update event</t>
   </si>
@@ -49,6 +49,30 @@
   </si>
   <si>
     <t>collect data(dynamic fields)</t>
+  </si>
+  <si>
+    <t>data reset after creating new action field</t>
+  </si>
+  <si>
+    <t>action new fields formatting</t>
+  </si>
+  <si>
+    <t>back buttons</t>
+  </si>
+  <si>
+    <t>action view all fields</t>
+  </si>
+  <si>
+    <t>what should happen when rest doesn't respond</t>
+  </si>
+  <si>
+    <t>defaulters</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>unique employee id check</t>
   </si>
 </sst>
 </file>
@@ -389,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,12 +483,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A5:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
report preparation and give-data link for employee
</commit_message>
<xml_diff>
--- a/product backlog.xlsx
+++ b/product backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>update event</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>unique employee id check</t>
+  </si>
+  <si>
+    <t>link for employee</t>
+  </si>
+  <si>
+    <t>Techincal</t>
+  </si>
+  <si>
+    <t>change required defaulters name as it is also used for report</t>
+  </si>
+  <si>
+    <t>check over all functionality</t>
+  </si>
+  <si>
+    <t>defaulters email ids</t>
+  </si>
+  <si>
+    <t>link copy for action, to share with employee</t>
+  </si>
+  <si>
+    <t>give data : action is displayed for all pax</t>
   </si>
 </sst>
 </file>
@@ -483,52 +504,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:A13"/>
+  <dimension ref="A5:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>